<commit_message>
taxi-out correction for EDDL, EIDW
</commit_message>
<xml_diff>
--- a/data/2015/RP2 - APT_TxOut_2015.xlsx
+++ b/data/2015/RP2 - APT_TxOut_2015.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="424">
   <si>
     <t>Data source</t>
   </si>
@@ -1276,6 +1276,15 @@
   </si>
   <si>
     <t>EDDH - SEP-DEC 2015 included, EVRA - MAY-DEC included, LEMD data correction for all 2015 due to processing error</t>
+  </si>
+  <si>
+    <t>21/MAR/2016</t>
+  </si>
+  <si>
+    <t>Clerical error - July 2015 data corrected</t>
+  </si>
+  <si>
+    <t>Clerical error - October 2015 data corrected</t>
   </si>
 </sst>
 </file>
@@ -2763,13 +2772,13 @@
         <v>92</v>
       </c>
       <c r="D18" s="23">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="E18" s="24">
-        <v>98389.0</v>
+        <v>98428.0</v>
       </c>
       <c r="F18" s="24">
-        <v>271000.0</v>
+        <v>269998.0</v>
       </c>
       <c r="G18" s="25">
         <v>8.66</v>
@@ -3361,16 +3370,16 @@
         <v>144</v>
       </c>
       <c r="D44" s="23">
-        <v>5.31</v>
+        <v>5.39</v>
       </c>
       <c r="E44" s="24">
-        <v>83777.0</v>
+        <v>84676.0</v>
       </c>
       <c r="F44" s="24">
-        <v>444977.0</v>
+        <v>456056.0</v>
       </c>
       <c r="G44" s="25">
-        <v>8.88</v>
+        <v>8.96</v>
       </c>
     </row>
     <row r="45" ht="12.75" customHeight="1">
@@ -6519,16 +6528,32 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
+      <c r="A4" s="45" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="47">
+        <v>2015.0</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
+      <c r="A5" s="45" t="s">
+        <v>421</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="47">
+        <v>2015.0</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="49"/>

</xml_diff>